<commit_message>
update: gitbook and pdf
</commit_message>
<xml_diff>
--- a/figures/redraw.xlsx
+++ b/figures/redraw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmc\pipetbooks\basic\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1442E6-7A3C-4EAB-882A-AEBD1CC1A451}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D53987-19AE-432A-BC9B-15CDABB8D0DB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8235" yWindow="4560" windowWidth="12150" windowHeight="11385" xr2:uid="{69547477-A67A-4239-A3A7-25BD2C2C0BE7}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="125">
   <si>
     <t>작업 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -430,6 +430,21 @@
   </si>
   <si>
     <t>11-fig-07</t>
+  </si>
+  <si>
+    <t>12-fig-01</t>
+  </si>
+  <si>
+    <t>13-fig-01</t>
+  </si>
+  <si>
+    <t>13-fig-02</t>
+  </si>
+  <si>
+    <t>13-fig-03</t>
+  </si>
+  <si>
+    <t>13-fig-06</t>
   </si>
 </sst>
 </file>
@@ -828,8 +843,8 @@
   </sheetPr>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1312,6 +1327,9 @@
       <c r="D31" t="s">
         <v>48</v>
       </c>
+      <c r="E31" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1">
@@ -1326,8 +1344,11 @@
       <c r="D32" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>130</v>
       </c>
@@ -1338,8 +1359,11 @@
       <c r="D33" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>131</v>
       </c>
@@ -1350,8 +1374,11 @@
       <c r="D34" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>133</v>
       </c>
@@ -1364,8 +1391,11 @@
       <c r="D35" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>134</v>
       </c>
@@ -1379,7 +1409,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>135</v>
       </c>
@@ -1391,7 +1421,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>156</v>
       </c>
@@ -1403,7 +1433,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>157</v>
       </c>
@@ -1415,7 +1445,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>159</v>
       </c>
@@ -1429,7 +1459,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>160</v>
       </c>
@@ -1441,7 +1471,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>161</v>
       </c>
@@ -1455,7 +1485,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>161</v>
       </c>
@@ -1469,7 +1499,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>162</v>
       </c>
@@ -1483,7 +1513,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>162</v>
       </c>
@@ -1497,7 +1527,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>166</v>
       </c>
@@ -1509,7 +1539,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>168</v>
       </c>
@@ -1521,7 +1551,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>169</v>
       </c>

</xml_diff>